<commit_message>
Faculty: Display Grades Table
</commit_message>
<xml_diff>
--- a/student-data-format.xlsx
+++ b/student-data-format.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="29">
   <si>
     <t>Student No</t>
   </si>
@@ -47,82 +47,70 @@
     <t>Subjects</t>
   </si>
   <si>
+    <t>Specialization</t>
+  </si>
+  <si>
+    <t>Program</t>
+  </si>
+  <si>
+    <t>Class Section</t>
+  </si>
+  <si>
+    <t>ANGELES, Patrick Agdeppa</t>
+  </si>
+  <si>
+    <t>BSIT</t>
+  </si>
+  <si>
+    <t>4th Year</t>
+  </si>
+  <si>
+    <t>Business Analytics</t>
+  </si>
+  <si>
+    <t>09662399839</t>
+  </si>
+  <si>
+    <t>BELANDRES, Marc Jason Variante</t>
+  </si>
+  <si>
+    <t>09772532723</t>
+  </si>
+  <si>
+    <t>BENAVENTE, Angelica Arceo</t>
+  </si>
+  <si>
+    <t>09488317041</t>
+  </si>
+  <si>
+    <t>BERNARDO, Jeanne Ruby Homelda</t>
+  </si>
+  <si>
+    <t>09750972256</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>Female</t>
+  </si>
+  <si>
+    <t>IT 401, IT 402, IT 403, CAP 402</t>
+  </si>
+  <si>
+    <t>patrick@bulsu.edu.ph</t>
+  </si>
+  <si>
+    <t>jason@gmail.com</t>
+  </si>
+  <si>
+    <t>angelica@gmail.com</t>
+  </si>
+  <si>
+    <t>jeanne@gmail.com</t>
+  </si>
+  <si>
     <t>4A</t>
-  </si>
-  <si>
-    <t>Specialization</t>
-  </si>
-  <si>
-    <t>Program</t>
-  </si>
-  <si>
-    <t>Class Section</t>
-  </si>
-  <si>
-    <t>ANGELES, Patrick Agdeppa</t>
-  </si>
-  <si>
-    <t>BSIT</t>
-  </si>
-  <si>
-    <t>4th Year</t>
-  </si>
-  <si>
-    <t>Business Analytics</t>
-  </si>
-  <si>
-    <t>09662399839</t>
-  </si>
-  <si>
-    <t>IT 401, IT 402, IT 403, CAP 401</t>
-  </si>
-  <si>
-    <t>BELANDRES, Marc Jason Variante</t>
-  </si>
-  <si>
-    <t>09772532723</t>
-  </si>
-  <si>
-    <t>BENAVENTE, Angelica Arceo</t>
-  </si>
-  <si>
-    <t>09488317041</t>
-  </si>
-  <si>
-    <t>BERNARDO, Jeanne Ruby Homelda</t>
-  </si>
-  <si>
-    <t>09750972256</t>
-  </si>
-  <si>
-    <t>Male</t>
-  </si>
-  <si>
-    <t>Female</t>
-  </si>
-  <si>
-    <t>IT 401, IT 402, IT 403, CAP 402</t>
-  </si>
-  <si>
-    <t>IT 401, IT 402, IT 403, CAP 403</t>
-  </si>
-  <si>
-    <t>IT 401, IT 402, IT 403, CAP 404</t>
-  </si>
-  <si>
-    <t>patrick@bulsu.edu.ph</t>
-  </si>
-  <si>
-    <t>jason@gmail.com</t>
-  </si>
-  <si>
-    <t>4B</t>
-  </si>
-  <si>
-    <t>4C</t>
-  </si>
-  <si>
-    <t>4D</t>
   </si>
 </sst>
 </file>
@@ -230,7 +218,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -271,6 +259,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -575,10 +566,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:J15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2:H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -591,7 +582,7 @@
     <col min="6" max="7" width="12" style="6" customWidth="1"/>
     <col min="8" max="8" width="12.42578125" style="6" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="17.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="29.42578125" style="9" customWidth="1"/>
+    <col min="10" max="10" width="65" style="9" bestFit="1" customWidth="1"/>
     <col min="11" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
@@ -612,16 +603,16 @@
         <v>5</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J1" s="5" t="s">
         <v>6</v>
@@ -632,31 +623,31 @@
         <v>2019115302</v>
       </c>
       <c r="B2" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="G2" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="J2" s="16" t="s">
         <v>23</v>
-      </c>
-      <c r="D2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="F2" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="H2" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="I2" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="J2" s="9" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -664,31 +655,31 @@
         <v>2019115088</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C3" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="J3" s="16" t="s">
         <v>23</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="E3" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="F3" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="G3" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="H3" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="I3" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="J3" s="9" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -696,29 +687,31 @@
         <v>2019117363</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="D4" s="3"/>
+        <v>22</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>26</v>
+      </c>
       <c r="E4" s="10" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F4" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="G4" s="11" t="s">
+      <c r="H4" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="I4" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="H4" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="I4" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="J4" s="9" t="s">
-        <v>26</v>
+      <c r="J4" s="16" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -726,30 +719,59 @@
         <v>2019115324</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="D5" s="3"/>
+        <v>22</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>27</v>
+      </c>
       <c r="E5" s="10" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F5" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="11" t="s">
+      <c r="H5" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="I5" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="I5" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="J5" s="9" t="s">
-        <v>27</v>
-      </c>
+      <c r="J5" s="16" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H7"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H8"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H9"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H10"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H11"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H12"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H13"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H14"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H15"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1 A3:A1048576">
@@ -760,8 +782,10 @@
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="D3" r:id="rId1"/>
+    <hyperlink ref="D4" r:id="rId2"/>
+    <hyperlink ref="D5" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>